<commit_message>
platemap submitted for RNA UTGSAF
</commit_message>
<xml_diff>
--- a/documentation/MRdiversitySampleSubmissionForm.xlsx
+++ b/documentation/MRdiversitySampleSubmissionForm.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssdon\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssdon\OneDrive\Documents\coral-DNA-RNA-lab-extractions\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B38BBE39-8962-4EC0-A1E8-C1226AC481E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA223A2E-5E5D-4D92-8F7A-2AA4AC07985C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60" yWindow="-60" windowWidth="20640" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample log" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="113">
   <si>
     <t xml:space="preserve">Lab Use Only </t>
   </si>
@@ -297,21 +297,88 @@
     <t>16s</t>
   </si>
   <si>
-    <t>15uL</t>
-  </si>
-  <si>
-    <t>water-blank</t>
-  </si>
-  <si>
     <t>DNA-blank</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>mock</t>
+  </si>
+  <si>
+    <t>blank</t>
+  </si>
+  <si>
+    <t>DNA</t>
+  </si>
+  <si>
+    <t>1-CA2a</t>
+  </si>
+  <si>
+    <t>1-CH2a</t>
+  </si>
+  <si>
+    <t>1-Ea</t>
+  </si>
+  <si>
+    <t>1-PA2a</t>
+  </si>
+  <si>
+    <t>1-PH1a</t>
+  </si>
+  <si>
+    <t>2-CA2a</t>
+  </si>
+  <si>
+    <t>2-CH1b</t>
+  </si>
+  <si>
+    <t>2-Ea</t>
+  </si>
+  <si>
+    <t>2-PA1b</t>
+  </si>
+  <si>
+    <t>2-PH2a</t>
+  </si>
+  <si>
+    <t>3-CA1b</t>
+  </si>
+  <si>
+    <t>3-CH2a</t>
+  </si>
+  <si>
+    <t>3-Eb</t>
+  </si>
+  <si>
+    <t>3-PA1a</t>
+  </si>
+  <si>
+    <t>3-PH1b</t>
+  </si>
+  <si>
+    <t>4-CA1a</t>
+  </si>
+  <si>
+    <t>4-CH1a</t>
+  </si>
+  <si>
+    <t>4-Ea</t>
+  </si>
+  <si>
+    <t>4-PA2a</t>
+  </si>
+  <si>
+    <t>4-PH1b</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -397,7 +464,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -464,8 +531,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -693,12 +766,58 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -792,15 +911,51 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -813,40 +968,16 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1245,10 +1376,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:L92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I92" sqref="A1:I92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1363,10 +1497,10 @@
       <c r="B12" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="59" t="s">
+      <c r="C12" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="60"/>
+      <c r="D12" s="52"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="29" t="s">
@@ -1375,50 +1509,50 @@
       <c r="B13" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="59" t="s">
+      <c r="C13" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="D13" s="60"/>
+      <c r="D13" s="52"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="2"/>
       <c r="B14" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="59" t="s">
+      <c r="C14" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="D14" s="60"/>
+      <c r="D14" s="52"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="2"/>
       <c r="B15" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="59" t="s">
+      <c r="C15" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="D15" s="60"/>
+      <c r="D15" s="52"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="2"/>
       <c r="B16" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="59" t="s">
+      <c r="C16" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="D16" s="60"/>
+      <c r="D16" s="52"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="2"/>
       <c r="B17" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="59" t="s">
+      <c r="C17" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="D17" s="60"/>
+      <c r="D17" s="52"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -1430,8 +1564,8 @@
       <c r="B18" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="59"/>
-      <c r="D18" s="60"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="52"/>
       <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.45">
@@ -1439,16 +1573,16 @@
       <c r="B19" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="67" t="s">
+      <c r="C19" s="54" t="s">
         <v>82</v>
       </c>
-      <c r="D19" s="58"/>
+      <c r="D19" s="55"/>
       <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="2"/>
-      <c r="C20" s="54"/>
-      <c r="D20" s="55"/>
+      <c r="C20" s="66"/>
+      <c r="D20" s="67"/>
       <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.45">
@@ -1456,8 +1590,8 @@
         <v>32</v>
       </c>
       <c r="B21" s="27"/>
-      <c r="C21" s="56"/>
-      <c r="D21" s="57"/>
+      <c r="C21" s="68"/>
+      <c r="D21" s="69"/>
       <c r="G21" s="10" t="s">
         <v>0</v>
       </c>
@@ -1470,10 +1604,10 @@
       <c r="B22" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="52" t="s">
+      <c r="C22" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="D22" s="53"/>
+      <c r="D22" s="60"/>
       <c r="G22" s="10"/>
       <c r="H22" s="1"/>
     </row>
@@ -1484,10 +1618,10 @@
       <c r="B23" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="52" t="s">
+      <c r="C23" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="D23" s="53"/>
+      <c r="D23" s="60"/>
       <c r="G23" s="10" t="s">
         <v>2</v>
       </c>
@@ -1497,40 +1631,40 @@
       <c r="B24" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="52" t="s">
+      <c r="C24" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="D24" s="53"/>
+      <c r="D24" s="60"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="17"/>
       <c r="B25" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="52" t="s">
+      <c r="C25" s="59" t="s">
         <v>79</v>
       </c>
-      <c r="D25" s="53"/>
+      <c r="D25" s="60"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="17"/>
       <c r="B26" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="52" t="s">
+      <c r="C26" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="D26" s="53"/>
+      <c r="D26" s="60"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="17"/>
       <c r="B27" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="64" t="s">
+      <c r="C27" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="D27" s="65"/>
+      <c r="D27" s="64"/>
       <c r="H27" s="10"/>
       <c r="I27" s="10"/>
     </row>
@@ -1539,8 +1673,8 @@
       <c r="B28" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="64"/>
-      <c r="D28" s="65"/>
+      <c r="C28" s="63"/>
+      <c r="D28" s="64"/>
       <c r="E28" t="s">
         <v>55</v>
       </c>
@@ -1551,10 +1685,10 @@
       <c r="B29" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C29" s="68" t="s">
+      <c r="C29" s="61" t="s">
         <v>82</v>
       </c>
-      <c r="D29" s="69"/>
+      <c r="D29" s="62"/>
       <c r="E29" t="s">
         <v>54</v>
       </c>
@@ -1586,7 +1720,7 @@
         <v>19</v>
       </c>
       <c r="C31" s="35">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D31" t="s">
         <v>17</v>
@@ -1594,7 +1728,9 @@
       <c r="E31" t="s">
         <v>72</v>
       </c>
-      <c r="G31" s="20"/>
+      <c r="G31" s="20" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" s="15" t="s">
@@ -1608,7 +1744,9 @@
       <c r="E32" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G32" s="20"/>
+      <c r="G32" s="20" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="33" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A33" s="40" t="s">
@@ -1626,7 +1764,9 @@
       <c r="E33" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G33" s="20"/>
+      <c r="G33" s="20" t="s">
+        <v>89</v>
+      </c>
       <c r="I33" t="s">
         <v>65</v>
       </c>
@@ -1642,7 +1782,9 @@
       <c r="E34" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G34" s="20"/>
+      <c r="G34" s="20" t="s">
+        <v>89</v>
+      </c>
       <c r="H34" t="s">
         <v>53</v>
       </c>
@@ -1664,7 +1806,9 @@
       <c r="E35" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G35" s="20"/>
+      <c r="G35" s="20" t="s">
+        <v>89</v>
+      </c>
       <c r="H35" t="s">
         <v>53</v>
       </c>
@@ -1681,7 +1825,9 @@
       <c r="E36" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G36" s="20"/>
+      <c r="G36" s="20" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A37" s="15" t="s">
@@ -1696,6 +1842,9 @@
       </c>
       <c r="E37" s="2" t="s">
         <v>64</v>
+      </c>
+      <c r="G37" s="70" t="s">
+        <v>89</v>
       </c>
       <c r="H37" t="s">
         <v>63</v>
@@ -1772,12 +1921,12 @@
       <c r="H42" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="I42" s="61" t="s">
+      <c r="I42" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="J42" s="62"/>
-      <c r="K42" s="62"/>
-      <c r="L42" s="62"/>
+      <c r="J42" s="57"/>
+      <c r="K42" s="57"/>
+      <c r="L42" s="57"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A43" s="42" t="s">
@@ -1802,12 +1951,12 @@
         <v>46</v>
       </c>
       <c r="H43" s="44"/>
-      <c r="I43" s="63" t="s">
+      <c r="I43" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="J43" s="63"/>
-      <c r="K43" s="63"/>
-      <c r="L43" s="63"/>
+      <c r="J43" s="58"/>
+      <c r="K43" s="58"/>
+      <c r="L43" s="58"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A44" s="45"/>
@@ -1818,17 +1967,17 @@
       <c r="F44" s="45"/>
       <c r="G44" s="45"/>
       <c r="H44" s="47"/>
-      <c r="I44" s="51"/>
-      <c r="J44" s="51"/>
-      <c r="K44" s="51"/>
-      <c r="L44" s="51"/>
+      <c r="I44" s="65"/>
+      <c r="J44" s="65"/>
+      <c r="K44" s="65"/>
+      <c r="L44" s="65"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A45" s="3" t="s">
-        <v>89</v>
+      <c r="A45" s="71" t="s">
+        <v>93</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>87</v>
@@ -1842,308 +1991,778 @@
       <c r="F45" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G45" s="3" t="s">
+      <c r="G45" s="3">
+        <v>20</v>
+      </c>
+      <c r="H45" s="4"/>
+      <c r="I45" s="73">
+        <v>21.4</v>
+      </c>
+      <c r="J45" s="74">
+        <v>21.4</v>
+      </c>
+      <c r="K45" s="74">
+        <v>21.4</v>
+      </c>
+      <c r="L45" s="75">
+        <v>21.4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A46" s="71" t="s">
+        <v>94</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G46" s="3">
+        <v>20</v>
+      </c>
+      <c r="H46" s="4"/>
+      <c r="I46" s="73">
+        <v>16</v>
+      </c>
+      <c r="J46" s="74">
+        <v>16</v>
+      </c>
+      <c r="K46" s="74">
+        <v>16</v>
+      </c>
+      <c r="L46" s="75">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A47" s="71" t="s">
+        <v>95</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G47" s="3">
+        <v>20</v>
+      </c>
+      <c r="H47" s="4"/>
+      <c r="I47" s="73">
+        <v>15.45</v>
+      </c>
+      <c r="J47" s="74">
+        <v>15.45</v>
+      </c>
+      <c r="K47" s="74">
+        <v>15.45</v>
+      </c>
+      <c r="L47" s="75">
+        <v>15.45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A48" s="71" t="s">
+        <v>96</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G48" s="3">
+        <v>20</v>
+      </c>
+      <c r="H48" s="4"/>
+      <c r="I48" s="73">
+        <v>21.1</v>
+      </c>
+      <c r="J48" s="74">
+        <v>21.1</v>
+      </c>
+      <c r="K48" s="74">
+        <v>21.1</v>
+      </c>
+      <c r="L48" s="75">
+        <v>21.1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A49" s="71" t="s">
+        <v>97</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G49" s="3">
+        <v>20</v>
+      </c>
+      <c r="H49" s="4"/>
+      <c r="I49" s="73">
+        <v>22.2</v>
+      </c>
+      <c r="J49" s="74">
+        <v>22.2</v>
+      </c>
+      <c r="K49" s="74">
+        <v>22.2</v>
+      </c>
+      <c r="L49" s="75">
+        <v>22.2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A50" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G50" s="3">
+        <v>20</v>
+      </c>
+      <c r="H50" s="4"/>
+      <c r="I50" s="73">
+        <v>19.350000000000001</v>
+      </c>
+      <c r="J50" s="74">
+        <v>19.350000000000001</v>
+      </c>
+      <c r="K50" s="74">
+        <v>19.350000000000001</v>
+      </c>
+      <c r="L50" s="75">
+        <v>19.350000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A51" s="71" t="s">
+        <v>99</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G51" s="3">
+        <v>20</v>
+      </c>
+      <c r="H51" s="4"/>
+      <c r="I51" s="73">
+        <v>9.2100000000000009</v>
+      </c>
+      <c r="J51" s="74">
+        <v>9.2100000000000009</v>
+      </c>
+      <c r="K51" s="74">
+        <v>9.2100000000000009</v>
+      </c>
+      <c r="L51" s="75">
+        <v>9.2100000000000009</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A52" s="71" t="s">
+        <v>100</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G52" s="3">
+        <v>20</v>
+      </c>
+      <c r="H52" s="4"/>
+      <c r="I52" s="73">
+        <v>13.9</v>
+      </c>
+      <c r="J52" s="74">
+        <v>13.9</v>
+      </c>
+      <c r="K52" s="74">
+        <v>13.9</v>
+      </c>
+      <c r="L52" s="75">
+        <v>13.9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A53" s="71" t="s">
+        <v>101</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G53" s="3">
+        <v>20</v>
+      </c>
+      <c r="H53" s="4"/>
+      <c r="I53" s="73">
+        <v>15.9</v>
+      </c>
+      <c r="J53" s="74">
+        <v>15.9</v>
+      </c>
+      <c r="K53" s="74">
+        <v>15.9</v>
+      </c>
+      <c r="L53" s="75">
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A54" s="71" t="s">
+        <v>102</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G54" s="3">
+        <v>20</v>
+      </c>
+      <c r="H54" s="4"/>
+      <c r="I54" s="73">
+        <v>19.299999999999997</v>
+      </c>
+      <c r="J54" s="74">
+        <v>19.299999999999997</v>
+      </c>
+      <c r="K54" s="74">
+        <v>19.299999999999997</v>
+      </c>
+      <c r="L54" s="75">
+        <v>19.299999999999997</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A55" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G55" s="3">
+        <v>20</v>
+      </c>
+      <c r="H55" s="4"/>
+      <c r="I55" s="73">
+        <v>19.350000000000001</v>
+      </c>
+      <c r="J55" s="74">
+        <v>19.350000000000001</v>
+      </c>
+      <c r="K55" s="74">
+        <v>19.350000000000001</v>
+      </c>
+      <c r="L55" s="75">
+        <v>19.350000000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A56" s="71" t="s">
+        <v>104</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G56" s="3">
+        <v>20</v>
+      </c>
+      <c r="H56" s="4"/>
+      <c r="I56" s="73">
+        <v>22.8</v>
+      </c>
+      <c r="J56" s="74">
+        <v>22.8</v>
+      </c>
+      <c r="K56" s="74">
+        <v>22.8</v>
+      </c>
+      <c r="L56" s="75">
+        <v>22.8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A57" s="71" t="s">
+        <v>105</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G57" s="3">
+        <v>20</v>
+      </c>
+      <c r="H57" s="4"/>
+      <c r="I57" s="73">
+        <v>17.3</v>
+      </c>
+      <c r="J57" s="74">
+        <v>17.3</v>
+      </c>
+      <c r="K57" s="74">
+        <v>17.3</v>
+      </c>
+      <c r="L57" s="75">
+        <v>17.3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A58" s="71" t="s">
+        <v>106</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G58" s="3">
+        <v>20</v>
+      </c>
+      <c r="H58" s="4"/>
+      <c r="I58" s="73">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="J58" s="74">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="K58" s="74">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="L58" s="75">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A59" s="71" t="s">
+        <v>107</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G59" s="3">
+        <v>20</v>
+      </c>
+      <c r="H59" s="4"/>
+      <c r="I59" s="73">
+        <v>18.5</v>
+      </c>
+      <c r="J59" s="74">
+        <v>18.5</v>
+      </c>
+      <c r="K59" s="74">
+        <v>18.5</v>
+      </c>
+      <c r="L59" s="75">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A60" s="71" t="s">
+        <v>108</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G60" s="3">
+        <v>20</v>
+      </c>
+      <c r="H60" s="4"/>
+      <c r="I60" s="73">
+        <v>21.4</v>
+      </c>
+      <c r="J60" s="74">
+        <v>21.4</v>
+      </c>
+      <c r="K60" s="74">
+        <v>21.4</v>
+      </c>
+      <c r="L60" s="75">
+        <v>21.4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A61" s="71" t="s">
+        <v>109</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G61" s="3">
+        <v>20</v>
+      </c>
+      <c r="H61" s="4"/>
+      <c r="I61" s="73">
+        <v>19.299999999999997</v>
+      </c>
+      <c r="J61" s="74">
+        <v>19.299999999999997</v>
+      </c>
+      <c r="K61" s="74">
+        <v>19.299999999999997</v>
+      </c>
+      <c r="L61" s="75">
+        <v>19.299999999999997</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A62" s="71" t="s">
+        <v>110</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G62" s="3">
+        <v>20</v>
+      </c>
+      <c r="H62" s="4"/>
+      <c r="I62" s="73">
+        <v>15.45</v>
+      </c>
+      <c r="J62" s="74">
+        <v>15.45</v>
+      </c>
+      <c r="K62" s="74">
+        <v>15.45</v>
+      </c>
+      <c r="L62" s="75">
+        <v>15.45</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A63" s="71" t="s">
+        <v>111</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G63" s="3">
+        <v>20</v>
+      </c>
+      <c r="H63" s="4"/>
+      <c r="I63" s="73">
+        <v>19</v>
+      </c>
+      <c r="J63" s="74">
+        <v>19</v>
+      </c>
+      <c r="K63" s="74">
+        <v>19</v>
+      </c>
+      <c r="L63" s="75">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A64" s="71" t="s">
+        <v>112</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G64" s="3">
+        <v>20</v>
+      </c>
+      <c r="H64" s="4"/>
+      <c r="I64" s="73">
+        <v>16.45</v>
+      </c>
+      <c r="J64" s="74">
+        <v>16.45</v>
+      </c>
+      <c r="K64" s="74">
+        <v>16.45</v>
+      </c>
+      <c r="L64" s="75">
+        <v>16.45</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A65" s="71" t="s">
+        <v>91</v>
+      </c>
+      <c r="B65" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="H45" s="4"/>
-      <c r="I45" s="66"/>
-      <c r="J45" s="66"/>
-      <c r="K45" s="66"/>
-      <c r="L45" s="66"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A46" s="3"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="4"/>
-      <c r="I46" s="66"/>
-      <c r="J46" s="66"/>
-      <c r="K46" s="66"/>
-      <c r="L46" s="66"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A47" s="3"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="4"/>
-      <c r="I47" s="66"/>
-      <c r="J47" s="66"/>
-      <c r="K47" s="66"/>
-      <c r="L47" s="66"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A48" s="3"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="66"/>
-      <c r="J48" s="66"/>
-      <c r="K48" s="66"/>
-      <c r="L48" s="66"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A49" s="3"/>
-      <c r="B49" s="5"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="4"/>
-      <c r="I49" s="66"/>
-      <c r="J49" s="66"/>
-      <c r="K49" s="66"/>
-      <c r="L49" s="66"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A50" s="3"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="4"/>
-      <c r="I50" s="66"/>
-      <c r="J50" s="66"/>
-      <c r="K50" s="66"/>
-      <c r="L50" s="66"/>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A51" s="3"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="4"/>
-      <c r="I51" s="66"/>
-      <c r="J51" s="66"/>
-      <c r="K51" s="66"/>
-      <c r="L51" s="66"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A52" s="3"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="4"/>
-      <c r="I52" s="66"/>
-      <c r="J52" s="66"/>
-      <c r="K52" s="66"/>
-      <c r="L52" s="66"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A53" s="3"/>
-      <c r="B53" s="5"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="4"/>
-      <c r="I53" s="66"/>
-      <c r="J53" s="66"/>
-      <c r="K53" s="66"/>
-      <c r="L53" s="66"/>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A54" s="3"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-      <c r="H54" s="4"/>
-      <c r="I54" s="66"/>
-      <c r="J54" s="66"/>
-      <c r="K54" s="66"/>
-      <c r="L54" s="66"/>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A55" s="3"/>
-      <c r="B55" s="5"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-      <c r="H55" s="4"/>
-      <c r="I55" s="66"/>
-      <c r="J55" s="66"/>
-      <c r="K55" s="66"/>
-      <c r="L55" s="66"/>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A56" s="3"/>
-      <c r="B56" s="5"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3"/>
-      <c r="H56" s="4"/>
-      <c r="I56" s="66"/>
-      <c r="J56" s="66"/>
-      <c r="K56" s="66"/>
-      <c r="L56" s="66"/>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A57" s="3"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
-      <c r="H57" s="4"/>
-      <c r="I57" s="66"/>
-      <c r="J57" s="66"/>
-      <c r="K57" s="66"/>
-      <c r="L57" s="66"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A58" s="3"/>
-      <c r="B58" s="5"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
-      <c r="H58" s="4"/>
-      <c r="I58" s="66"/>
-      <c r="J58" s="66"/>
-      <c r="K58" s="66"/>
-      <c r="L58" s="66"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A59" s="3"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
-      <c r="H59" s="4"/>
-      <c r="I59" s="66"/>
-      <c r="J59" s="66"/>
-      <c r="K59" s="66"/>
-      <c r="L59" s="66"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A60" s="3"/>
-      <c r="B60" s="5"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
-      <c r="G60" s="3"/>
-      <c r="H60" s="4"/>
-      <c r="I60" s="66"/>
-      <c r="J60" s="66"/>
-      <c r="K60" s="66"/>
-      <c r="L60" s="66"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A61" s="3"/>
-      <c r="B61" s="5"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
-      <c r="G61" s="3"/>
-      <c r="H61" s="4"/>
-      <c r="I61" s="66"/>
-      <c r="J61" s="66"/>
-      <c r="K61" s="66"/>
-      <c r="L61" s="66"/>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A62" s="3"/>
-      <c r="B62" s="5"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
-      <c r="G62" s="3"/>
-      <c r="H62" s="4"/>
-      <c r="I62" s="66"/>
-      <c r="J62" s="66"/>
-      <c r="K62" s="66"/>
-      <c r="L62" s="66"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A63" s="3"/>
-      <c r="B63" s="5"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-      <c r="G63" s="3"/>
-      <c r="H63" s="4"/>
-      <c r="I63" s="66"/>
-      <c r="J63" s="66"/>
-      <c r="K63" s="66"/>
-      <c r="L63" s="66"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A64" s="3"/>
-      <c r="B64" s="5"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
-      <c r="G64" s="3"/>
-      <c r="H64" s="4"/>
-      <c r="I64" s="66"/>
-      <c r="J64" s="66"/>
-      <c r="K64" s="66"/>
-      <c r="L64" s="66"/>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A65" s="3"/>
-      <c r="B65" s="5"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
-      <c r="G65" s="3"/>
+      <c r="C65" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G65" s="3">
+        <v>20</v>
+      </c>
       <c r="H65" s="4"/>
-      <c r="I65" s="66"/>
-      <c r="J65" s="66"/>
-      <c r="K65" s="66"/>
-      <c r="L65" s="66"/>
+      <c r="I65" s="73">
+        <v>0</v>
+      </c>
+      <c r="J65" s="74">
+        <v>0</v>
+      </c>
+      <c r="K65" s="74">
+        <v>0</v>
+      </c>
+      <c r="L65" s="75">
+        <v>0</v>
+      </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A66" s="3"/>
-      <c r="B66" s="5"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
-      <c r="G66" s="3"/>
+      <c r="A66" s="72" t="s">
+        <v>90</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G66" s="3">
+        <v>20</v>
+      </c>
       <c r="H66" s="4"/>
-      <c r="I66" s="66"/>
-      <c r="J66" s="66"/>
-      <c r="K66" s="66"/>
-      <c r="L66" s="66"/>
+      <c r="I66" s="73">
+        <v>22</v>
+      </c>
+      <c r="J66" s="74">
+        <v>22</v>
+      </c>
+      <c r="K66" s="74">
+        <v>22</v>
+      </c>
+      <c r="L66" s="75">
+        <v>22</v>
+      </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A67" s="3"/>
@@ -2154,10 +2773,10 @@
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
       <c r="H67" s="4"/>
-      <c r="I67" s="66"/>
-      <c r="J67" s="66"/>
-      <c r="K67" s="66"/>
-      <c r="L67" s="66"/>
+      <c r="I67" s="53"/>
+      <c r="J67" s="53"/>
+      <c r="K67" s="53"/>
+      <c r="L67" s="53"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A68" s="3"/>
@@ -2168,10 +2787,10 @@
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
       <c r="H68" s="4"/>
-      <c r="I68" s="66"/>
-      <c r="J68" s="66"/>
-      <c r="K68" s="66"/>
-      <c r="L68" s="66"/>
+      <c r="I68" s="53"/>
+      <c r="J68" s="53"/>
+      <c r="K68" s="53"/>
+      <c r="L68" s="53"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A69" s="3"/>
@@ -2182,10 +2801,10 @@
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
       <c r="H69" s="4"/>
-      <c r="I69" s="66"/>
-      <c r="J69" s="66"/>
-      <c r="K69" s="66"/>
-      <c r="L69" s="66"/>
+      <c r="I69" s="53"/>
+      <c r="J69" s="53"/>
+      <c r="K69" s="53"/>
+      <c r="L69" s="53"/>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A70" s="3"/>
@@ -2196,10 +2815,10 @@
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
       <c r="H70" s="4"/>
-      <c r="I70" s="66"/>
-      <c r="J70" s="66"/>
-      <c r="K70" s="66"/>
-      <c r="L70" s="66"/>
+      <c r="I70" s="53"/>
+      <c r="J70" s="53"/>
+      <c r="K70" s="53"/>
+      <c r="L70" s="53"/>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A71" s="3"/>
@@ -2210,10 +2829,10 @@
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>
       <c r="H71" s="4"/>
-      <c r="I71" s="66"/>
-      <c r="J71" s="66"/>
-      <c r="K71" s="66"/>
-      <c r="L71" s="66"/>
+      <c r="I71" s="53"/>
+      <c r="J71" s="53"/>
+      <c r="K71" s="53"/>
+      <c r="L71" s="53"/>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A72" s="3"/>
@@ -2224,10 +2843,10 @@
       <c r="F72" s="3"/>
       <c r="G72" s="3"/>
       <c r="H72" s="4"/>
-      <c r="I72" s="66"/>
-      <c r="J72" s="66"/>
-      <c r="K72" s="66"/>
-      <c r="L72" s="66"/>
+      <c r="I72" s="53"/>
+      <c r="J72" s="53"/>
+      <c r="K72" s="53"/>
+      <c r="L72" s="53"/>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A73" s="3"/>
@@ -2238,10 +2857,10 @@
       <c r="F73" s="3"/>
       <c r="G73" s="3"/>
       <c r="H73" s="4"/>
-      <c r="I73" s="66"/>
-      <c r="J73" s="66"/>
-      <c r="K73" s="66"/>
-      <c r="L73" s="66"/>
+      <c r="I73" s="53"/>
+      <c r="J73" s="53"/>
+      <c r="K73" s="53"/>
+      <c r="L73" s="53"/>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A74" s="3"/>
@@ -2252,10 +2871,10 @@
       <c r="F74" s="3"/>
       <c r="G74" s="3"/>
       <c r="H74" s="4"/>
-      <c r="I74" s="66"/>
-      <c r="J74" s="66"/>
-      <c r="K74" s="66"/>
-      <c r="L74" s="66"/>
+      <c r="I74" s="53"/>
+      <c r="J74" s="53"/>
+      <c r="K74" s="53"/>
+      <c r="L74" s="53"/>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A75" s="3"/>
@@ -2266,10 +2885,10 @@
       <c r="F75" s="3"/>
       <c r="G75" s="3"/>
       <c r="H75" s="4"/>
-      <c r="I75" s="66"/>
-      <c r="J75" s="66"/>
-      <c r="K75" s="66"/>
-      <c r="L75" s="66"/>
+      <c r="I75" s="53"/>
+      <c r="J75" s="53"/>
+      <c r="K75" s="53"/>
+      <c r="L75" s="53"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A76" s="3"/>
@@ -2280,10 +2899,10 @@
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
       <c r="H76" s="4"/>
-      <c r="I76" s="66"/>
-      <c r="J76" s="66"/>
-      <c r="K76" s="66"/>
-      <c r="L76" s="66"/>
+      <c r="I76" s="53"/>
+      <c r="J76" s="53"/>
+      <c r="K76" s="53"/>
+      <c r="L76" s="53"/>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A77" s="3"/>
@@ -2294,10 +2913,10 @@
       <c r="F77" s="3"/>
       <c r="G77" s="3"/>
       <c r="H77" s="4"/>
-      <c r="I77" s="66"/>
-      <c r="J77" s="66"/>
-      <c r="K77" s="66"/>
-      <c r="L77" s="66"/>
+      <c r="I77" s="53"/>
+      <c r="J77" s="53"/>
+      <c r="K77" s="53"/>
+      <c r="L77" s="53"/>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A78" s="3"/>
@@ -2308,10 +2927,10 @@
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
       <c r="H78" s="4"/>
-      <c r="I78" s="66"/>
-      <c r="J78" s="66"/>
-      <c r="K78" s="66"/>
-      <c r="L78" s="66"/>
+      <c r="I78" s="53"/>
+      <c r="J78" s="53"/>
+      <c r="K78" s="53"/>
+      <c r="L78" s="53"/>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A79" s="3"/>
@@ -2322,10 +2941,10 @@
       <c r="F79" s="3"/>
       <c r="G79" s="3"/>
       <c r="H79" s="4"/>
-      <c r="I79" s="66"/>
-      <c r="J79" s="66"/>
-      <c r="K79" s="66"/>
-      <c r="L79" s="66"/>
+      <c r="I79" s="53"/>
+      <c r="J79" s="53"/>
+      <c r="K79" s="53"/>
+      <c r="L79" s="53"/>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A80" s="3"/>
@@ -2336,10 +2955,10 @@
       <c r="F80" s="3"/>
       <c r="G80" s="3"/>
       <c r="H80" s="4"/>
-      <c r="I80" s="66"/>
-      <c r="J80" s="66"/>
-      <c r="K80" s="66"/>
-      <c r="L80" s="66"/>
+      <c r="I80" s="53"/>
+      <c r="J80" s="53"/>
+      <c r="K80" s="53"/>
+      <c r="L80" s="53"/>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A81" s="3"/>
@@ -2350,10 +2969,10 @@
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
       <c r="H81" s="4"/>
-      <c r="I81" s="66"/>
-      <c r="J81" s="66"/>
-      <c r="K81" s="66"/>
-      <c r="L81" s="66"/>
+      <c r="I81" s="53"/>
+      <c r="J81" s="53"/>
+      <c r="K81" s="53"/>
+      <c r="L81" s="53"/>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A82" s="3"/>
@@ -2364,10 +2983,10 @@
       <c r="F82" s="3"/>
       <c r="G82" s="3"/>
       <c r="H82" s="4"/>
-      <c r="I82" s="66"/>
-      <c r="J82" s="66"/>
-      <c r="K82" s="66"/>
-      <c r="L82" s="66"/>
+      <c r="I82" s="53"/>
+      <c r="J82" s="53"/>
+      <c r="K82" s="53"/>
+      <c r="L82" s="53"/>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A83" s="3"/>
@@ -2378,10 +2997,10 @@
       <c r="F83" s="3"/>
       <c r="G83" s="3"/>
       <c r="H83" s="4"/>
-      <c r="I83" s="66"/>
-      <c r="J83" s="66"/>
-      <c r="K83" s="66"/>
-      <c r="L83" s="66"/>
+      <c r="I83" s="53"/>
+      <c r="J83" s="53"/>
+      <c r="K83" s="53"/>
+      <c r="L83" s="53"/>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A84" s="3"/>
@@ -2392,10 +3011,10 @@
       <c r="F84" s="3"/>
       <c r="G84" s="3"/>
       <c r="H84" s="4"/>
-      <c r="I84" s="66"/>
-      <c r="J84" s="66"/>
-      <c r="K84" s="66"/>
-      <c r="L84" s="66"/>
+      <c r="I84" s="53"/>
+      <c r="J84" s="53"/>
+      <c r="K84" s="53"/>
+      <c r="L84" s="53"/>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A85" s="3"/>
@@ -2406,10 +3025,10 @@
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
       <c r="H85" s="4"/>
-      <c r="I85" s="66"/>
-      <c r="J85" s="66"/>
-      <c r="K85" s="66"/>
-      <c r="L85" s="66"/>
+      <c r="I85" s="53"/>
+      <c r="J85" s="53"/>
+      <c r="K85" s="53"/>
+      <c r="L85" s="53"/>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A86" s="3"/>
@@ -2420,10 +3039,10 @@
       <c r="F86" s="3"/>
       <c r="G86" s="3"/>
       <c r="H86" s="4"/>
-      <c r="I86" s="66"/>
-      <c r="J86" s="66"/>
-      <c r="K86" s="66"/>
-      <c r="L86" s="66"/>
+      <c r="I86" s="53"/>
+      <c r="J86" s="53"/>
+      <c r="K86" s="53"/>
+      <c r="L86" s="53"/>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A87" s="3"/>
@@ -2434,10 +3053,10 @@
       <c r="F87" s="3"/>
       <c r="G87" s="3"/>
       <c r="H87" s="4"/>
-      <c r="I87" s="66"/>
-      <c r="J87" s="66"/>
-      <c r="K87" s="66"/>
-      <c r="L87" s="66"/>
+      <c r="I87" s="53"/>
+      <c r="J87" s="53"/>
+      <c r="K87" s="53"/>
+      <c r="L87" s="53"/>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A88" s="3"/>
@@ -2448,10 +3067,10 @@
       <c r="F88" s="3"/>
       <c r="G88" s="3"/>
       <c r="H88" s="4"/>
-      <c r="I88" s="66"/>
-      <c r="J88" s="66"/>
-      <c r="K88" s="66"/>
-      <c r="L88" s="66"/>
+      <c r="I88" s="53"/>
+      <c r="J88" s="53"/>
+      <c r="K88" s="53"/>
+      <c r="L88" s="53"/>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A89" s="3"/>
@@ -2462,10 +3081,10 @@
       <c r="F89" s="3"/>
       <c r="G89" s="3"/>
       <c r="H89" s="4"/>
-      <c r="I89" s="66"/>
-      <c r="J89" s="66"/>
-      <c r="K89" s="66"/>
-      <c r="L89" s="66"/>
+      <c r="I89" s="53"/>
+      <c r="J89" s="53"/>
+      <c r="K89" s="53"/>
+      <c r="L89" s="53"/>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A90" s="3"/>
@@ -2476,10 +3095,10 @@
       <c r="F90" s="3"/>
       <c r="G90" s="3"/>
       <c r="H90" s="4"/>
-      <c r="I90" s="66"/>
-      <c r="J90" s="66"/>
-      <c r="K90" s="66"/>
-      <c r="L90" s="66"/>
+      <c r="I90" s="53"/>
+      <c r="J90" s="53"/>
+      <c r="K90" s="53"/>
+      <c r="L90" s="53"/>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A91" s="3"/>
@@ -2490,10 +3109,10 @@
       <c r="F91" s="3"/>
       <c r="G91" s="3"/>
       <c r="H91" s="4"/>
-      <c r="I91" s="66"/>
-      <c r="J91" s="66"/>
-      <c r="K91" s="66"/>
-      <c r="L91" s="66"/>
+      <c r="I91" s="53"/>
+      <c r="J91" s="53"/>
+      <c r="K91" s="53"/>
+      <c r="L91" s="53"/>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A92" s="3"/>
@@ -2504,66 +3123,18 @@
       <c r="F92" s="3"/>
       <c r="G92" s="3"/>
       <c r="H92" s="4"/>
-      <c r="I92" s="66"/>
-      <c r="J92" s="66"/>
-      <c r="K92" s="66"/>
-      <c r="L92" s="66"/>
+      <c r="I92" s="53"/>
+      <c r="J92" s="53"/>
+      <c r="K92" s="53"/>
+      <c r="L92" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="I80:L80"/>
-    <mergeCell ref="I81:L81"/>
-    <mergeCell ref="I82:L82"/>
-    <mergeCell ref="I83:L83"/>
-    <mergeCell ref="I84:L84"/>
-    <mergeCell ref="I90:L90"/>
-    <mergeCell ref="I91:L91"/>
-    <mergeCell ref="I92:L92"/>
-    <mergeCell ref="I85:L85"/>
-    <mergeCell ref="I86:L86"/>
-    <mergeCell ref="I87:L87"/>
-    <mergeCell ref="I88:L88"/>
-    <mergeCell ref="I89:L89"/>
-    <mergeCell ref="I77:L77"/>
-    <mergeCell ref="I78:L78"/>
-    <mergeCell ref="I79:L79"/>
-    <mergeCell ref="I70:L70"/>
-    <mergeCell ref="I71:L71"/>
-    <mergeCell ref="I72:L72"/>
-    <mergeCell ref="I73:L73"/>
-    <mergeCell ref="I74:L74"/>
-    <mergeCell ref="I75:L75"/>
-    <mergeCell ref="I76:L76"/>
-    <mergeCell ref="I65:L65"/>
-    <mergeCell ref="I66:L66"/>
-    <mergeCell ref="I67:L67"/>
-    <mergeCell ref="I68:L68"/>
-    <mergeCell ref="I69:L69"/>
-    <mergeCell ref="I60:L60"/>
-    <mergeCell ref="I61:L61"/>
-    <mergeCell ref="I62:L62"/>
-    <mergeCell ref="I63:L63"/>
-    <mergeCell ref="I64:L64"/>
-    <mergeCell ref="I55:L55"/>
-    <mergeCell ref="I56:L56"/>
-    <mergeCell ref="I57:L57"/>
-    <mergeCell ref="I58:L58"/>
-    <mergeCell ref="I59:L59"/>
-    <mergeCell ref="I50:L50"/>
-    <mergeCell ref="I51:L51"/>
-    <mergeCell ref="I52:L52"/>
-    <mergeCell ref="I53:L53"/>
-    <mergeCell ref="I54:L54"/>
-    <mergeCell ref="I45:L45"/>
-    <mergeCell ref="I46:L46"/>
-    <mergeCell ref="I47:L47"/>
-    <mergeCell ref="I48:L48"/>
-    <mergeCell ref="I49:L49"/>
+    <mergeCell ref="I44:L44"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C17:D17"/>
@@ -2575,18 +3146,69 @@
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="C25:D25"/>
-    <mergeCell ref="I44:L44"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="I45:L45"/>
+    <mergeCell ref="I46:L46"/>
+    <mergeCell ref="I47:L47"/>
+    <mergeCell ref="I48:L48"/>
+    <mergeCell ref="I49:L49"/>
+    <mergeCell ref="I50:L50"/>
+    <mergeCell ref="I51:L51"/>
+    <mergeCell ref="I52:L52"/>
+    <mergeCell ref="I53:L53"/>
+    <mergeCell ref="I54:L54"/>
+    <mergeCell ref="I55:L55"/>
+    <mergeCell ref="I56:L56"/>
+    <mergeCell ref="I57:L57"/>
+    <mergeCell ref="I58:L58"/>
+    <mergeCell ref="I59:L59"/>
+    <mergeCell ref="I60:L60"/>
+    <mergeCell ref="I61:L61"/>
+    <mergeCell ref="I62:L62"/>
+    <mergeCell ref="I63:L63"/>
+    <mergeCell ref="I64:L64"/>
+    <mergeCell ref="I65:L65"/>
+    <mergeCell ref="I66:L66"/>
+    <mergeCell ref="I67:L67"/>
+    <mergeCell ref="I68:L68"/>
+    <mergeCell ref="I69:L69"/>
+    <mergeCell ref="I77:L77"/>
+    <mergeCell ref="I78:L78"/>
+    <mergeCell ref="I79:L79"/>
+    <mergeCell ref="I70:L70"/>
+    <mergeCell ref="I71:L71"/>
+    <mergeCell ref="I72:L72"/>
+    <mergeCell ref="I73:L73"/>
+    <mergeCell ref="I74:L74"/>
+    <mergeCell ref="I75:L75"/>
+    <mergeCell ref="I76:L76"/>
+    <mergeCell ref="I90:L90"/>
+    <mergeCell ref="I91:L91"/>
+    <mergeCell ref="I92:L92"/>
+    <mergeCell ref="I85:L85"/>
+    <mergeCell ref="I86:L86"/>
+    <mergeCell ref="I87:L87"/>
+    <mergeCell ref="I88:L88"/>
+    <mergeCell ref="I89:L89"/>
+    <mergeCell ref="I80:L80"/>
+    <mergeCell ref="I81:L81"/>
+    <mergeCell ref="I82:L82"/>
+    <mergeCell ref="I83:L83"/>
+    <mergeCell ref="I84:L84"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C12:D12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="C19" r:id="rId2" xr:uid="{F0B3E98D-EB9B-4C6C-B08D-E24BD74D5405}"/>
   </hyperlinks>
-  <pageMargins left="0.13" right="0.13" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="59" fitToHeight="0" orientation="landscape" r:id="rId3"/>
+  <headerFooter>
+    <oddHeader>&amp;F</oddHeader>
+  </headerFooter>
   <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>